<commit_message>
Update todas issues 18/05/2024
</commit_message>
<xml_diff>
--- a/public/Relatorio_ConfigCarros.xlsx
+++ b/public/Relatorio_ConfigCarros.xlsx
@@ -10,14 +10,14 @@
     <sheet name="ConfigCarros" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ConfigCarros'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ConfigCarros'!$A$1:$I$2</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>nome</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>Data de Cadastro</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>Ativo</t>
+  </si>
+  <si>
+    <t>17/05/2024 - 11:06:28</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,8 +429,37 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:I2"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>